<commit_message>
use async await appendFile
</commit_message>
<xml_diff>
--- a/node/crawler/ximalaya/output.xlsx
+++ b/node/crawler/ximalaya/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F745"/>
+  <dimension ref="A1:F749"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15280,9 +15280,89 @@
         <v>否</v>
       </c>
     </row>
+    <row r="746">
+      <c r="A746">
+        <v>35350539</v>
+      </c>
+      <c r="B746" t="str">
+        <v>硅谷钢铁侠：埃隆·马斯克的冒险人生|雷军、丁磊、周鸿祎力荐</v>
+      </c>
+      <c r="C746" t="str">
+        <v>是</v>
+      </c>
+      <c r="D746">
+        <v>22</v>
+      </c>
+      <c r="E746" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F746" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747">
+        <v>38534851</v>
+      </c>
+      <c r="B747" t="str">
+        <v>好的经济学（2019年诺贝尔经济学奖得主新作）</v>
+      </c>
+      <c r="C747" t="str">
+        <v>是</v>
+      </c>
+      <c r="D747">
+        <v>35</v>
+      </c>
+      <c r="E747" t="str">
+        <v>商业财经</v>
+      </c>
+      <c r="F747" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748">
+        <v>38534389</v>
+      </c>
+      <c r="B748" t="str">
+        <v>十年一觉电影梦：李安传</v>
+      </c>
+      <c r="C748" t="str">
+        <v>是</v>
+      </c>
+      <c r="D748">
+        <v>41</v>
+      </c>
+      <c r="E748" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F748" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749">
+        <v>38536383</v>
+      </c>
+      <c r="B749" t="str">
+        <v>社交媒体简史：从莎草纸到互联网</v>
+      </c>
+      <c r="C749" t="str">
+        <v>是</v>
+      </c>
+      <c r="D749">
+        <v>25</v>
+      </c>
+      <c r="E749" t="str">
+        <v>人文</v>
+      </c>
+      <c r="F749" t="str">
+        <v>否</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F745"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F749"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write sh to excaute all
</commit_message>
<xml_diff>
--- a/node/crawler/ximalaya/output.xlsx
+++ b/node/crawler/ximalaya/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2019"/>
+  <dimension ref="A1:F2022"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -40760,9 +40760,69 @@
         <v>否</v>
       </c>
     </row>
+    <row r="2020">
+      <c r="A2020">
+        <v>32650457</v>
+      </c>
+      <c r="B2020" t="str">
+        <v>一剑独尊（20年玄幻大作 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C2020" t="str">
+        <v>否</v>
+      </c>
+      <c r="D2020">
+        <v>1224</v>
+      </c>
+      <c r="E2020" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F2020" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="2021">
+      <c r="A2021">
+        <v>31887842</v>
+      </c>
+      <c r="B2021" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C2021" t="str">
+        <v>否</v>
+      </c>
+      <c r="D2021">
+        <v>1383</v>
+      </c>
+      <c r="E2021" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F2021" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="2022">
+      <c r="A2022">
+        <v>34220825</v>
+      </c>
+      <c r="B2022" t="str">
+        <v>遮天（辰东作品，头陀渊&amp;小桃红精品双播）</v>
+      </c>
+      <c r="C2022" t="str">
+        <v>否</v>
+      </c>
+      <c r="D2022">
+        <v>685</v>
+      </c>
+      <c r="E2022" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F2022" t="str">
+        <v>否</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2019"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2022"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update free album download
</commit_message>
<xml_diff>
--- a/node/crawler/ximalaya/output.xlsx
+++ b/node/crawler/ximalaya/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F977"/>
+  <dimension ref="A1:F1139"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -19920,9 +19920,3249 @@
         <v>否</v>
       </c>
     </row>
+    <row r="978">
+      <c r="A978">
+        <v>8274546</v>
+      </c>
+      <c r="B978" t="str">
+        <v>周建龙演播-《五大贼王1-7合集》</v>
+      </c>
+      <c r="C978" t="str">
+        <v>是</v>
+      </c>
+      <c r="D978">
+        <v>449</v>
+      </c>
+      <c r="E978" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F978" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979">
+        <v>29135574</v>
+      </c>
+      <c r="B979" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C979" t="str">
+        <v>否</v>
+      </c>
+      <c r="D979">
+        <v>123</v>
+      </c>
+      <c r="E979" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F979" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980">
+        <v>40544228</v>
+      </c>
+      <c r="B980" t="str">
+        <v>捍宝|民国盗墓探险 抗日热血（周建龙播讲）</v>
+      </c>
+      <c r="C980" t="str">
+        <v>否</v>
+      </c>
+      <c r="D980">
+        <v>247</v>
+      </c>
+      <c r="E980" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F980" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981">
+        <v>12517524</v>
+      </c>
+      <c r="B981" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C981" t="str">
+        <v>否</v>
+      </c>
+      <c r="D981">
+        <v>143</v>
+      </c>
+      <c r="E981" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F981" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982">
+        <v>37407947</v>
+      </c>
+      <c r="B982" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C982" t="str">
+        <v>否</v>
+      </c>
+      <c r="D982">
+        <v>833</v>
+      </c>
+      <c r="E982" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F982" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983">
+        <v>40121646</v>
+      </c>
+      <c r="B983" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C983" t="str">
+        <v>否</v>
+      </c>
+      <c r="D983">
+        <v>290</v>
+      </c>
+      <c r="E983" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F983" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984">
+        <v>30816438</v>
+      </c>
+      <c r="B984" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C984" t="str">
+        <v>否</v>
+      </c>
+      <c r="D984">
+        <v>56</v>
+      </c>
+      <c r="E984" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F984" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985">
+        <v>30222680</v>
+      </c>
+      <c r="B985" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C985" t="str">
+        <v>否</v>
+      </c>
+      <c r="D985">
+        <v>1506</v>
+      </c>
+      <c r="E985" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F985" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986">
+        <v>5949372</v>
+      </c>
+      <c r="B986" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C986" t="str">
+        <v>否</v>
+      </c>
+      <c r="D986">
+        <v>1433</v>
+      </c>
+      <c r="E986" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F986" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987">
+        <v>20134156</v>
+      </c>
+      <c r="B987" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C987" t="str">
+        <v>否</v>
+      </c>
+      <c r="D987">
+        <v>1569</v>
+      </c>
+      <c r="E987" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F987" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988">
+        <v>33476331</v>
+      </c>
+      <c r="B988" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C988" t="str">
+        <v>否</v>
+      </c>
+      <c r="D988">
+        <v>734</v>
+      </c>
+      <c r="E988" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F988" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989">
+        <v>29135574</v>
+      </c>
+      <c r="B989" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C989" t="str">
+        <v>否</v>
+      </c>
+      <c r="D989">
+        <v>123</v>
+      </c>
+      <c r="E989" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F989" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990">
+        <v>40544228</v>
+      </c>
+      <c r="B990" t="str">
+        <v>捍宝|民国盗墓探险 抗日热血（周建龙播讲）</v>
+      </c>
+      <c r="C990" t="str">
+        <v>否</v>
+      </c>
+      <c r="D990">
+        <v>247</v>
+      </c>
+      <c r="E990" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F990" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991">
+        <v>12517524</v>
+      </c>
+      <c r="B991" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C991" t="str">
+        <v>否</v>
+      </c>
+      <c r="D991">
+        <v>144</v>
+      </c>
+      <c r="E991" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F991" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992">
+        <v>37407947</v>
+      </c>
+      <c r="B992" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C992" t="str">
+        <v>否</v>
+      </c>
+      <c r="D992">
+        <v>848</v>
+      </c>
+      <c r="E992" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F992" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993">
+        <v>40121646</v>
+      </c>
+      <c r="B993" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C993" t="str">
+        <v>否</v>
+      </c>
+      <c r="D993">
+        <v>296</v>
+      </c>
+      <c r="E993" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F993" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994">
+        <v>30816438</v>
+      </c>
+      <c r="B994" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C994" t="str">
+        <v>否</v>
+      </c>
+      <c r="D994">
+        <v>56</v>
+      </c>
+      <c r="E994" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F994" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995">
+        <v>30222680</v>
+      </c>
+      <c r="B995" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C995" t="str">
+        <v>否</v>
+      </c>
+      <c r="D995">
+        <v>1507</v>
+      </c>
+      <c r="E995" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F995" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996">
+        <v>5949372</v>
+      </c>
+      <c r="B996" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C996" t="str">
+        <v>否</v>
+      </c>
+      <c r="D996">
+        <v>1433</v>
+      </c>
+      <c r="E996" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F996" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997">
+        <v>20134156</v>
+      </c>
+      <c r="B997" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C997" t="str">
+        <v>否</v>
+      </c>
+      <c r="D997">
+        <v>1578</v>
+      </c>
+      <c r="E997" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F997" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998">
+        <v>33476331</v>
+      </c>
+      <c r="B998" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C998" t="str">
+        <v>否</v>
+      </c>
+      <c r="D998">
+        <v>737</v>
+      </c>
+      <c r="E998" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F998" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999">
+        <v>32650457</v>
+      </c>
+      <c r="B999" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C999" t="str">
+        <v>否</v>
+      </c>
+      <c r="D999">
+        <v>1698</v>
+      </c>
+      <c r="E999" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F999" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000">
+        <v>25010802</v>
+      </c>
+      <c r="B1000" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1000" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1000">
+        <v>2136</v>
+      </c>
+      <c r="E1000" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1000" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001">
+        <v>38160002</v>
+      </c>
+      <c r="B1001" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1001" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1001">
+        <v>625</v>
+      </c>
+      <c r="E1001" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1001" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002">
+        <v>41152884</v>
+      </c>
+      <c r="B1002" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1002" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1002">
+        <v>639</v>
+      </c>
+      <c r="E1002" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1002" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003">
+        <v>40121646</v>
+      </c>
+      <c r="B1003" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1003" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1003">
+        <v>296</v>
+      </c>
+      <c r="E1003" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1003" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004">
+        <v>31887842</v>
+      </c>
+      <c r="B1004" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C1004" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1004">
+        <v>1626</v>
+      </c>
+      <c r="E1004" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1004" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005">
+        <v>34220825</v>
+      </c>
+      <c r="B1005" t="str">
+        <v>遮天（辰东作品，头陀渊&amp;小桃红精品双播）</v>
+      </c>
+      <c r="C1005" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1005">
+        <v>952</v>
+      </c>
+      <c r="E1005" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1005" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006">
+        <v>39361268</v>
+      </c>
+      <c r="B1006" t="str">
+        <v>无案不眠（现言悬疑精品多人剧）</v>
+      </c>
+      <c r="C1006" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1006">
+        <v>896</v>
+      </c>
+      <c r="E1006" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1006" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007">
+        <v>33541329</v>
+      </c>
+      <c r="B1007" t="str">
+        <v>少帅你老婆又跑了|民国言情多人</v>
+      </c>
+      <c r="C1007" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1007">
+        <v>1432</v>
+      </c>
+      <c r="E1007" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1007" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008">
+        <v>29135574</v>
+      </c>
+      <c r="B1008" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1008" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1008">
+        <v>123</v>
+      </c>
+      <c r="E1008" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1008" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009">
+        <v>40544228</v>
+      </c>
+      <c r="B1009" t="str">
+        <v>捍宝|民国盗墓探险 抗日热血（周建龙播讲）</v>
+      </c>
+      <c r="C1009" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1009">
+        <v>247</v>
+      </c>
+      <c r="E1009" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1009" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010">
+        <v>12517524</v>
+      </c>
+      <c r="B1010" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1010" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1010">
+        <v>144</v>
+      </c>
+      <c r="E1010" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1010" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011">
+        <v>37407947</v>
+      </c>
+      <c r="B1011" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1011" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1011">
+        <v>849</v>
+      </c>
+      <c r="E1011" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1011" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012">
+        <v>25167841</v>
+      </c>
+      <c r="B1012" t="str">
+        <v>实用人格手册：读懂自己与他人的必备指南</v>
+      </c>
+      <c r="C1012" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1012">
+        <v>39</v>
+      </c>
+      <c r="E1012" t="str">
+        <v>个人成长</v>
+      </c>
+      <c r="F1012" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013">
+        <v>35535482</v>
+      </c>
+      <c r="B1013" t="str">
+        <v>霍乱时期的爱情 | 马尔克斯代表作，杨晨、吴凌云演播</v>
+      </c>
+      <c r="C1013" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1013">
+        <v>76</v>
+      </c>
+      <c r="E1013" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1013" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014">
+        <v>29135574</v>
+      </c>
+      <c r="B1014" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1014" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1014">
+        <v>124</v>
+      </c>
+      <c r="E1014" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1014" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015">
+        <v>12517524</v>
+      </c>
+      <c r="B1015" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1015" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1015">
+        <v>146</v>
+      </c>
+      <c r="E1015" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1015" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016">
+        <v>29135574</v>
+      </c>
+      <c r="B1016" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1016" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1016">
+        <v>124</v>
+      </c>
+      <c r="E1016" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1016" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017">
+        <v>12517524</v>
+      </c>
+      <c r="B1017" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1017" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1017">
+        <v>146</v>
+      </c>
+      <c r="E1017" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1017" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018">
+        <v>29135574</v>
+      </c>
+      <c r="B1018" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1018" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1018">
+        <v>124</v>
+      </c>
+      <c r="E1018" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1018" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019">
+        <v>12517524</v>
+      </c>
+      <c r="B1019" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1019" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1019">
+        <v>146</v>
+      </c>
+      <c r="E1019" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1019" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020">
+        <v>29135574</v>
+      </c>
+      <c r="B1020" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1020" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1020">
+        <v>124</v>
+      </c>
+      <c r="E1020" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1020" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021">
+        <v>12517524</v>
+      </c>
+      <c r="B1021" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1021" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1021">
+        <v>146</v>
+      </c>
+      <c r="E1021" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1021" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022">
+        <v>29135574</v>
+      </c>
+      <c r="B1022" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1022" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1022">
+        <v>124</v>
+      </c>
+      <c r="E1022" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1022" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023">
+        <v>12517524</v>
+      </c>
+      <c r="B1023" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1023" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1023">
+        <v>146</v>
+      </c>
+      <c r="E1023" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1023" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024">
+        <v>29135574</v>
+      </c>
+      <c r="B1024" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1024" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1024">
+        <v>124</v>
+      </c>
+      <c r="E1024" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1024" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025">
+        <v>12517524</v>
+      </c>
+      <c r="B1025" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1025" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1025">
+        <v>146</v>
+      </c>
+      <c r="E1025" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1025" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026">
+        <v>37407947</v>
+      </c>
+      <c r="B1026" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1026" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1026">
+        <v>897</v>
+      </c>
+      <c r="E1026" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1026" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027">
+        <v>40121646</v>
+      </c>
+      <c r="B1027" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1027" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1027">
+        <v>314</v>
+      </c>
+      <c r="E1027" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1027" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028">
+        <v>30816438</v>
+      </c>
+      <c r="B1028" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1028" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1028">
+        <v>59</v>
+      </c>
+      <c r="E1028" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1028" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029">
+        <v>30222680</v>
+      </c>
+      <c r="B1029" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1029" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1029">
+        <v>1511</v>
+      </c>
+      <c r="E1029" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1029" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030">
+        <v>5949372</v>
+      </c>
+      <c r="B1030" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1030" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1030">
+        <v>1435</v>
+      </c>
+      <c r="E1030" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1030" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031">
+        <v>29135574</v>
+      </c>
+      <c r="B1031" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1031" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1031">
+        <v>124</v>
+      </c>
+      <c r="E1031" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1031" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032">
+        <v>12517524</v>
+      </c>
+      <c r="B1032" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1032" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1032">
+        <v>147</v>
+      </c>
+      <c r="E1032" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1032" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033">
+        <v>37407947</v>
+      </c>
+      <c r="B1033" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1033" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1033">
+        <v>907</v>
+      </c>
+      <c r="E1033" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1033" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034">
+        <v>40121646</v>
+      </c>
+      <c r="B1034" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1034" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1034">
+        <v>314</v>
+      </c>
+      <c r="E1034" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1034" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035">
+        <v>30816438</v>
+      </c>
+      <c r="B1035" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1035" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1035">
+        <v>59</v>
+      </c>
+      <c r="E1035" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1035" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036">
+        <v>30222680</v>
+      </c>
+      <c r="B1036" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1036" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1036">
+        <v>1511</v>
+      </c>
+      <c r="E1036" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1036" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037">
+        <v>5949372</v>
+      </c>
+      <c r="B1037" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1037" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1037">
+        <v>1435</v>
+      </c>
+      <c r="E1037" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1037" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038">
+        <v>43964846</v>
+      </c>
+      <c r="B1038" t="str">
+        <v>老梁故事汇主讲人丨处世绝学29招丨职场高情商，教你好好说话</v>
+      </c>
+      <c r="C1038" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1038">
+        <v>13</v>
+      </c>
+      <c r="E1038" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1038" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039">
+        <v>29135574</v>
+      </c>
+      <c r="B1039" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1039" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1039">
+        <v>124</v>
+      </c>
+      <c r="E1039" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1039" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040">
+        <v>12517524</v>
+      </c>
+      <c r="B1040" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1040" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1040">
+        <v>147</v>
+      </c>
+      <c r="E1040" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1040" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041">
+        <v>37407947</v>
+      </c>
+      <c r="B1041" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1041" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1041">
+        <v>907</v>
+      </c>
+      <c r="E1041" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1041" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042">
+        <v>40121646</v>
+      </c>
+      <c r="B1042" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1042" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1042">
+        <v>314</v>
+      </c>
+      <c r="E1042" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1042" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043">
+        <v>30816438</v>
+      </c>
+      <c r="B1043" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1043" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1043">
+        <v>59</v>
+      </c>
+      <c r="E1043" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1043" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044">
+        <v>30222680</v>
+      </c>
+      <c r="B1044" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1044" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1044">
+        <v>1511</v>
+      </c>
+      <c r="E1044" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1044" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045">
+        <v>5949372</v>
+      </c>
+      <c r="B1045" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1045" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1045">
+        <v>1435</v>
+      </c>
+      <c r="E1045" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1045" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046">
+        <v>20134156</v>
+      </c>
+      <c r="B1046" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1046" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1046">
+        <v>1641</v>
+      </c>
+      <c r="E1046" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1046" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047">
+        <v>33476331</v>
+      </c>
+      <c r="B1047" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1047" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1047">
+        <v>758</v>
+      </c>
+      <c r="E1047" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1047" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048">
+        <v>29135574</v>
+      </c>
+      <c r="B1048" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1048" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1048">
+        <v>124</v>
+      </c>
+      <c r="E1048" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1048" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049">
+        <v>12517524</v>
+      </c>
+      <c r="B1049" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1049" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1049">
+        <v>147</v>
+      </c>
+      <c r="E1049" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1049" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050">
+        <v>37407947</v>
+      </c>
+      <c r="B1050" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1050" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1050">
+        <v>907</v>
+      </c>
+      <c r="E1050" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1050" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051">
+        <v>40121646</v>
+      </c>
+      <c r="B1051" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1051" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1051">
+        <v>314</v>
+      </c>
+      <c r="E1051" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1051" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052">
+        <v>30816438</v>
+      </c>
+      <c r="B1052" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1052" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1052">
+        <v>59</v>
+      </c>
+      <c r="E1052" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1052" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053">
+        <v>30222680</v>
+      </c>
+      <c r="B1053" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1053" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1053">
+        <v>1511</v>
+      </c>
+      <c r="E1053" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1053" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054">
+        <v>5949372</v>
+      </c>
+      <c r="B1054" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1054" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1054">
+        <v>1435</v>
+      </c>
+      <c r="E1054" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1054" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055">
+        <v>20134156</v>
+      </c>
+      <c r="B1055" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1055" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1055">
+        <v>1647</v>
+      </c>
+      <c r="E1055" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1055" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056">
+        <v>33476331</v>
+      </c>
+      <c r="B1056" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1056" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1056">
+        <v>760</v>
+      </c>
+      <c r="E1056" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1056" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057">
+        <v>32650457</v>
+      </c>
+      <c r="B1057" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1057" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1057">
+        <v>1750</v>
+      </c>
+      <c r="E1057" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1057" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058">
+        <v>25010802</v>
+      </c>
+      <c r="B1058" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1058" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1058">
+        <v>2160</v>
+      </c>
+      <c r="E1058" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1058" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059">
+        <v>38160002</v>
+      </c>
+      <c r="B1059" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1059" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1059">
+        <v>662</v>
+      </c>
+      <c r="E1059" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1059" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060">
+        <v>40121646</v>
+      </c>
+      <c r="B1060" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1060" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1060">
+        <v>314</v>
+      </c>
+      <c r="E1060" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1060" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061">
+        <v>29135574</v>
+      </c>
+      <c r="B1061" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1061" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1061">
+        <v>124</v>
+      </c>
+      <c r="E1061" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1061" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062">
+        <v>12517524</v>
+      </c>
+      <c r="B1062" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1062" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1062">
+        <v>147</v>
+      </c>
+      <c r="E1062" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1062" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063">
+        <v>37407947</v>
+      </c>
+      <c r="B1063" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1063" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1063">
+        <v>907</v>
+      </c>
+      <c r="E1063" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1063" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064">
+        <v>40121646</v>
+      </c>
+      <c r="B1064" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1064" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1064">
+        <v>314</v>
+      </c>
+      <c r="E1064" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1064" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065">
+        <v>30816438</v>
+      </c>
+      <c r="B1065" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1065" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1065">
+        <v>59</v>
+      </c>
+      <c r="E1065" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1065" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066">
+        <v>30222680</v>
+      </c>
+      <c r="B1066" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1066" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1066">
+        <v>1511</v>
+      </c>
+      <c r="E1066" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1066" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067">
+        <v>5949372</v>
+      </c>
+      <c r="B1067" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1067" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1067">
+        <v>1435</v>
+      </c>
+      <c r="E1067" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1067" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068">
+        <v>20134156</v>
+      </c>
+      <c r="B1068" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1068" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1068">
+        <v>1647</v>
+      </c>
+      <c r="E1068" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1068" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069">
+        <v>33476331</v>
+      </c>
+      <c r="B1069" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1069" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1069">
+        <v>760</v>
+      </c>
+      <c r="E1069" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1069" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070">
+        <v>32650457</v>
+      </c>
+      <c r="B1070" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1070" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1070">
+        <v>1750</v>
+      </c>
+      <c r="E1070" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1070" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071">
+        <v>25010802</v>
+      </c>
+      <c r="B1071" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1071" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1071">
+        <v>2160</v>
+      </c>
+      <c r="E1071" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1071" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072">
+        <v>38160002</v>
+      </c>
+      <c r="B1072" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1072" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1072">
+        <v>662</v>
+      </c>
+      <c r="E1072" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1072" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073">
+        <v>40121646</v>
+      </c>
+      <c r="B1073" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1073" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1073">
+        <v>314</v>
+      </c>
+      <c r="E1073" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1073" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074">
+        <v>41152884</v>
+      </c>
+      <c r="B1074" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1074" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1074">
+        <v>750</v>
+      </c>
+      <c r="E1074" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1074" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075">
+        <v>34220825</v>
+      </c>
+      <c r="B1075" t="str">
+        <v>遮天（辰东作品，头陀渊&amp;小桃红精品双播）</v>
+      </c>
+      <c r="C1075" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1075">
+        <v>1021</v>
+      </c>
+      <c r="E1075" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1075" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076">
+        <v>31887842</v>
+      </c>
+      <c r="B1076" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C1076" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1076">
+        <v>1672</v>
+      </c>
+      <c r="E1076" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1076" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077">
+        <v>29135574</v>
+      </c>
+      <c r="B1077" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1077" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1077">
+        <v>124</v>
+      </c>
+      <c r="E1077" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1077" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078">
+        <v>12517524</v>
+      </c>
+      <c r="B1078" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1078" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1078">
+        <v>147</v>
+      </c>
+      <c r="E1078" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1078" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079">
+        <v>37407947</v>
+      </c>
+      <c r="B1079" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1079" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1079">
+        <v>917</v>
+      </c>
+      <c r="E1079" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1079" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080">
+        <v>40121646</v>
+      </c>
+      <c r="B1080" t="str">
+        <v>三体（全集）| 有声小说，刘慈欣作品，王明军演播</v>
+      </c>
+      <c r="C1080" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1080">
+        <v>314</v>
+      </c>
+      <c r="E1080" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1080" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081">
+        <v>30816438</v>
+      </c>
+      <c r="B1081" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1081" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1081">
+        <v>59</v>
+      </c>
+      <c r="E1081" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1081" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082">
+        <v>30222680</v>
+      </c>
+      <c r="B1082" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1082" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1082">
+        <v>1511</v>
+      </c>
+      <c r="E1082" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1082" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083">
+        <v>5949372</v>
+      </c>
+      <c r="B1083" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1083" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1083">
+        <v>1435</v>
+      </c>
+      <c r="E1083" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1083" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084">
+        <v>20134156</v>
+      </c>
+      <c r="B1084" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1084" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1084">
+        <v>1650</v>
+      </c>
+      <c r="E1084" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1084" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085">
+        <v>33476331</v>
+      </c>
+      <c r="B1085" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1085" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1085">
+        <v>762</v>
+      </c>
+      <c r="E1085" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1085" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086">
+        <v>32650457</v>
+      </c>
+      <c r="B1086" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1086" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1086">
+        <v>1752</v>
+      </c>
+      <c r="E1086" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1086" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087">
+        <v>25010802</v>
+      </c>
+      <c r="B1087" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1087" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1087">
+        <v>2161</v>
+      </c>
+      <c r="E1087" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1087" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088">
+        <v>41152884</v>
+      </c>
+      <c r="B1088" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1088" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1088">
+        <v>756</v>
+      </c>
+      <c r="E1088" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1088" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089">
+        <v>38160002</v>
+      </c>
+      <c r="B1089" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1089" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1089">
+        <v>664</v>
+      </c>
+      <c r="E1089" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1089" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090">
+        <v>31887842</v>
+      </c>
+      <c r="B1090" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C1090" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1090">
+        <v>1676</v>
+      </c>
+      <c r="E1090" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1090" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091">
+        <v>34220825</v>
+      </c>
+      <c r="B1091" t="str">
+        <v>遮天（辰东作品，头陀渊&amp;小桃红精品双播）</v>
+      </c>
+      <c r="C1091" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1091">
+        <v>1024</v>
+      </c>
+      <c r="E1091" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1091" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092">
+        <v>19095902</v>
+      </c>
+      <c r="B1092" t="str">
+        <v>圣墟【头陀渊&amp;小桃红】遮天后传</v>
+      </c>
+      <c r="C1092" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1092">
+        <v>2227</v>
+      </c>
+      <c r="E1092" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1092" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093">
+        <v>24075975</v>
+      </c>
+      <c r="B1093" t="str">
+        <v>医学博士的心脑训练课【SMART】</v>
+      </c>
+      <c r="C1093" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1093">
+        <v>21</v>
+      </c>
+      <c r="E1093" t="str">
+        <v>教育培训</v>
+      </c>
+      <c r="F1093" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094">
+        <v>29135574</v>
+      </c>
+      <c r="B1094" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1094" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1094">
+        <v>124</v>
+      </c>
+      <c r="E1094" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1094" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095">
+        <v>12517524</v>
+      </c>
+      <c r="B1095" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1095" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1095">
+        <v>147</v>
+      </c>
+      <c r="E1095" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1095" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096">
+        <v>37407947</v>
+      </c>
+      <c r="B1096" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1096" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1096">
+        <v>922</v>
+      </c>
+      <c r="E1096" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1096" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097">
+        <v>30816438</v>
+      </c>
+      <c r="B1097" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1097" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1097">
+        <v>60</v>
+      </c>
+      <c r="E1097" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1097" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098">
+        <v>30222680</v>
+      </c>
+      <c r="B1098" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1098" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1098">
+        <v>1511</v>
+      </c>
+      <c r="E1098" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1098" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099">
+        <v>5949372</v>
+      </c>
+      <c r="B1099" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1099" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1099">
+        <v>1435</v>
+      </c>
+      <c r="E1099" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1099" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100">
+        <v>20134156</v>
+      </c>
+      <c r="B1100" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1100" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1100">
+        <v>1656</v>
+      </c>
+      <c r="E1100" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1100" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101">
+        <v>33476331</v>
+      </c>
+      <c r="B1101" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1101" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1101">
+        <v>764</v>
+      </c>
+      <c r="E1101" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1101" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102">
+        <v>32650457</v>
+      </c>
+      <c r="B1102" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1102" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1102">
+        <v>1756</v>
+      </c>
+      <c r="E1102" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1102" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103">
+        <v>25010802</v>
+      </c>
+      <c r="B1103" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1103" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1103">
+        <v>2163</v>
+      </c>
+      <c r="E1103" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1103" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104">
+        <v>41152884</v>
+      </c>
+      <c r="B1104" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1104" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1104">
+        <v>756</v>
+      </c>
+      <c r="E1104" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1104" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105">
+        <v>38160002</v>
+      </c>
+      <c r="B1105" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1105" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1105">
+        <v>669</v>
+      </c>
+      <c r="E1105" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1105" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106">
+        <v>31887842</v>
+      </c>
+      <c r="B1106" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C1106" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1106">
+        <v>1680</v>
+      </c>
+      <c r="E1106" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1106" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107">
+        <v>29135574</v>
+      </c>
+      <c r="B1107" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1107" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1107">
+        <v>124</v>
+      </c>
+      <c r="E1107" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1107" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108">
+        <v>12517524</v>
+      </c>
+      <c r="B1108" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1108" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1108">
+        <v>147</v>
+      </c>
+      <c r="E1108" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1108" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109">
+        <v>37407947</v>
+      </c>
+      <c r="B1109" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1109" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1109">
+        <v>927</v>
+      </c>
+      <c r="E1109" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1109" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110">
+        <v>30816438</v>
+      </c>
+      <c r="B1110" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1110" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1110">
+        <v>60</v>
+      </c>
+      <c r="E1110" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1110" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111">
+        <v>30222680</v>
+      </c>
+      <c r="B1111" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1111" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1111">
+        <v>1511</v>
+      </c>
+      <c r="E1111" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1111" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112">
+        <v>5949372</v>
+      </c>
+      <c r="B1112" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1112" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1112">
+        <v>1435</v>
+      </c>
+      <c r="E1112" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1112" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113">
+        <v>20134156</v>
+      </c>
+      <c r="B1113" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1113" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1113">
+        <v>1659</v>
+      </c>
+      <c r="E1113" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1113" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114">
+        <v>33476331</v>
+      </c>
+      <c r="B1114" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1114" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1114">
+        <v>764</v>
+      </c>
+      <c r="E1114" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1114" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115">
+        <v>32650457</v>
+      </c>
+      <c r="B1115" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1115" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1115">
+        <v>1758</v>
+      </c>
+      <c r="E1115" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1115" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116">
+        <v>25010802</v>
+      </c>
+      <c r="B1116" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1116" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1116">
+        <v>2163</v>
+      </c>
+      <c r="E1116" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1116" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117">
+        <v>41152884</v>
+      </c>
+      <c r="B1117" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1117" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1117">
+        <v>756</v>
+      </c>
+      <c r="E1117" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1117" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118">
+        <v>38160002</v>
+      </c>
+      <c r="B1118" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1118" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1118">
+        <v>669</v>
+      </c>
+      <c r="E1118" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1118" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119">
+        <v>16576596</v>
+      </c>
+      <c r="B1119" t="str">
+        <v>四世同堂 | 李野墨演播 老舍经典</v>
+      </c>
+      <c r="C1119" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1119">
+        <v>100</v>
+      </c>
+      <c r="E1119" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1119" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120">
+        <v>29135574</v>
+      </c>
+      <c r="B1120" t="str">
+        <v>神奇的a阿尔法脑波音乐 |雨声催眠减压 潜意识右脑开发</v>
+      </c>
+      <c r="C1120" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1120">
+        <v>125</v>
+      </c>
+      <c r="E1120" t="str">
+        <v>音乐</v>
+      </c>
+      <c r="F1120" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121">
+        <v>12517524</v>
+      </c>
+      <c r="B1121" t="str">
+        <v>王玥波播讲：雍正剑侠图·第七部</v>
+      </c>
+      <c r="C1121" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1121">
+        <v>148</v>
+      </c>
+      <c r="E1121" t="str">
+        <v>相声评书</v>
+      </c>
+      <c r="F1121" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122">
+        <v>37407947</v>
+      </c>
+      <c r="B1122" t="str">
+        <v>都市狂兵（双播精配）热血爽文 | 限时免费</v>
+      </c>
+      <c r="C1122" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1122">
+        <v>927</v>
+      </c>
+      <c r="E1122" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1122" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123">
+        <v>30816438</v>
+      </c>
+      <c r="B1123" t="str">
+        <v>三体（全六季）| 精品广播剧，刘慈欣著</v>
+      </c>
+      <c r="C1123" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1123">
+        <v>60</v>
+      </c>
+      <c r="E1123" t="str">
+        <v>广播剧</v>
+      </c>
+      <c r="F1123" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124">
+        <v>30222680</v>
+      </c>
+      <c r="B1124" t="str">
+        <v>老街中的痞子（爆更版）-VIP免费</v>
+      </c>
+      <c r="C1124" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1124">
+        <v>1511</v>
+      </c>
+      <c r="E1124" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1124" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125">
+        <v>5949372</v>
+      </c>
+      <c r="B1125" t="str">
+        <v>逆天邪神</v>
+      </c>
+      <c r="C1125" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1125">
+        <v>1435</v>
+      </c>
+      <c r="E1125" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1125" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126">
+        <v>20134156</v>
+      </c>
+      <c r="B1126" t="str">
+        <v>伏天氏（多人录制版）</v>
+      </c>
+      <c r="C1126" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1126">
+        <v>1662</v>
+      </c>
+      <c r="E1126" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1126" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127">
+        <v>33476331</v>
+      </c>
+      <c r="B1127" t="str">
+        <v>上门龙婿|至尊龙婿叶辰萧初然</v>
+      </c>
+      <c r="C1127" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1127">
+        <v>766</v>
+      </c>
+      <c r="E1127" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1127" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128">
+        <v>32650457</v>
+      </c>
+      <c r="B1128" t="str">
+        <v>一剑独尊（叶玄叶灵 | 有声的紫襟 | 男女双播）</v>
+      </c>
+      <c r="C1128" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1128">
+        <v>1760</v>
+      </c>
+      <c r="E1128" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1128" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129">
+        <v>25010802</v>
+      </c>
+      <c r="B1129" t="str">
+        <v>最佳女婿|火爆都市异能多人剧（喜马拉雅铁三角出品）</v>
+      </c>
+      <c r="C1129" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1129">
+        <v>2165</v>
+      </c>
+      <c r="E1129" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1129" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130">
+        <v>41152884</v>
+      </c>
+      <c r="B1130" t="str">
+        <v>盗墓手札丨有声的紫襟（盗墓笔记基友版）</v>
+      </c>
+      <c r="C1130" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1130">
+        <v>756</v>
+      </c>
+      <c r="E1130" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1130" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131">
+        <v>38160002</v>
+      </c>
+      <c r="B1131" t="str">
+        <v>庆余年【全三季】古风&amp;权谋（同名影视原著 | 精品多人剧）</v>
+      </c>
+      <c r="C1131" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1131">
+        <v>671</v>
+      </c>
+      <c r="E1131" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1131" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132">
+        <v>31887842</v>
+      </c>
+      <c r="B1132" t="str">
+        <v>超级女婿|又名: 豪婿（上门女婿韩三千）</v>
+      </c>
+      <c r="C1132" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1132">
+        <v>1682</v>
+      </c>
+      <c r="E1132" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1132" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133">
+        <v>37522647</v>
+      </c>
+      <c r="B1133" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1133" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1133">
+        <v>16</v>
+      </c>
+      <c r="E1133" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1133" t="str">
+        <v>是</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134">
+        <v>44955514</v>
+      </c>
+      <c r="B1134" t="str">
+        <v>一寸师|小人物的悲喜起落|黄梵著</v>
+      </c>
+      <c r="C1134" t="str">
+        <v>是</v>
+      </c>
+      <c r="D1134">
+        <v>27</v>
+      </c>
+      <c r="E1134" t="str">
+        <v>有声书</v>
+      </c>
+      <c r="F1134" t="str">
+        <v>否</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135">
+        <v>37522647</v>
+      </c>
+      <c r="B1135" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1135" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1135">
+        <v>16</v>
+      </c>
+      <c r="E1135" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1135" t="str">
+        <v>是</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136">
+        <v>37522647</v>
+      </c>
+      <c r="B1136" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1136" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1136">
+        <v>16</v>
+      </c>
+      <c r="E1136" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1136" t="str">
+        <v>是</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137">
+        <v>37522647</v>
+      </c>
+      <c r="B1137" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1137" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1137">
+        <v>16</v>
+      </c>
+      <c r="E1137" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1137" t="str">
+        <v>是</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138">
+        <v>37522647</v>
+      </c>
+      <c r="B1138" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1138" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1138">
+        <v>16</v>
+      </c>
+      <c r="E1138" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1138" t="str">
+        <v>是</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139">
+        <v>37522647</v>
+      </c>
+      <c r="B1139" t="str">
+        <v>《随园食单》白话文【有文稿】</v>
+      </c>
+      <c r="C1139" t="str">
+        <v>否</v>
+      </c>
+      <c r="D1139">
+        <v>16</v>
+      </c>
+      <c r="E1139" t="str">
+        <v>历史</v>
+      </c>
+      <c r="F1139" t="str">
+        <v>是</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F977"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F1139"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>